<commit_message>
added new question data
</commit_message>
<xml_diff>
--- a/src/test/resources/gpt.xlsx
+++ b/src/test/resources/gpt.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\git\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E197521-00C6-4E82-A909-63435A7668F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{61DEAD93-6817-4D7B-A98F-3ADCFB91D971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +11,7 @@
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>S.No</t>
   </si>
@@ -42,34 +38,37 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Create Java interview questions covering Core Java, OOPs, Collections, Exceptions, Java 8, and Multithreading.</t>
-  </si>
-  <si>
-    <t>Create Selenium WebDriver interview questions covering locators, waits, alerts, frames, windows, Actions class, JavaScriptExecutor, POM, and Selenium Grid.</t>
-  </si>
-  <si>
-    <t>Create TestNG interview questions covering annotations, assertions, DataProvider, testng.xml, parallel execution, and listeners.</t>
-  </si>
-  <si>
-    <t>Create Maven interview questions covering pom.xml structure, dependencies, build lifecycle, profiles, and Surefire/Failsafe plugins.</t>
-  </si>
-  <si>
-    <t>Create API testing interview questions covering REST principles, HTTP methods, status codes, authentication, request/response validation, and Rest Assured.</t>
-  </si>
-  <si>
-    <t>Include basic, intermediate, and advanced level questions for each technology.</t>
-  </si>
-  <si>
-    <t>Mix theoretical, scenario-based, and practical questions.Focus on real-world automation framework design and best practices.</t>
-  </si>
-  <si>
-    <t>Target candidates with 3–8 years of QA automation experience.Output questions in a clean, line-by-line, serial-numbered format.</t>
-  </si>
-  <si>
-    <t>Do not include explanations—only questions.This format is concise, structured, and LLM-friendly.</t>
-  </si>
-  <si>
     <t>gpt-4.1-mini</t>
+  </si>
+  <si>
+    <t>Create Java interview questions covering Core Java, OOPs, Collections, Exceptions, Java 8, and Multithreading. Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Create Java interview progarms covering Core Java, OOPs, Collections, Exceptions, Java 8, and Multithreading.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Create Selenium WebDriver interview questions covering locators, waits, alerts, frames, windows, Actions class, JavaScriptExecutor, POM, and Selenium Grid.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Create TestNG interview questions covering annotations, assertions, DataProvider, testng.xml, parallel execution, and listeners. Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Create Maven interview questions covering pom.xml structure, dependencies, build lifecycle, profiles, and Surefire/Failsafe plugins.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Create API testing interview questions covering REST principles, HTTP methods, status codes, authentication, request/response validation, and Rest Assured.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Include basic, intermediate, and advanced level questions for each technology.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Mix theoretical, scenario-based, and practical questions.Focus on real-world automation framework design and best practices.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Target candidates with 3–8 years of QA automation experience.Output questions in a clean, line-by-line, serial-numbered format.  Note: Always provide the question in serial number format</t>
+  </si>
+  <si>
+    <t>Do not include explanations—only questions.This format is concise, structured, and LLM-friendly.  Note: Always provide the question in serial number format</t>
   </si>
 </sst>
 </file>
@@ -412,7 +411,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -438,7 +437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -446,10 +445,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -460,13 +459,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -474,13 +473,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -488,10 +487,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -502,13 +501,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -516,13 +515,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -530,10 +529,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -544,13 +543,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -558,10 +557,24 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
+    </row>
+    <row r="11" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>